<commit_message>
Code for final colours
</commit_message>
<xml_diff>
--- a/colours.xlsx
+++ b/colours.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="45">
   <si>
     <t>Colour Combinations</t>
   </si>
@@ -101,24 +101,6 @@
     <t xml:space="preserve">Broad and Narrow </t>
   </si>
   <si>
-    <t>U-UV W</t>
-  </si>
-  <si>
-    <t>U-OII</t>
-  </si>
-  <si>
-    <t>B-H_Beta</t>
-  </si>
-  <si>
-    <t>V-OIII</t>
-  </si>
-  <si>
-    <t>V-H_Alpha</t>
-  </si>
-  <si>
-    <t>V-SII</t>
-  </si>
-  <si>
     <t>3 Dimensions</t>
   </si>
   <si>
@@ -126,13 +108,64 @@
   </si>
   <si>
     <t>* May not be meaningful</t>
+  </si>
+  <si>
+    <t>c-c-c Plots</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kmeans </t>
+  </si>
+  <si>
+    <t>Meanshift</t>
+  </si>
+  <si>
+    <t>Affinity</t>
+  </si>
+  <si>
+    <t>HMS</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>UV W - U</t>
+  </si>
+  <si>
+    <t>U - OII</t>
+  </si>
+  <si>
+    <t>B- H_Beta</t>
+  </si>
+  <si>
+    <t>OIII - V</t>
+  </si>
+  <si>
+    <t>B - V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B - I </t>
+  </si>
+  <si>
+    <t>V - I</t>
+  </si>
+  <si>
+    <t>U - B</t>
+  </si>
+  <si>
+    <t>H_Alpha - I</t>
+  </si>
+  <si>
+    <t>SII - I</t>
+  </si>
+  <si>
+    <t>U - V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -156,16 +189,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="29">
+  <borders count="33">
     <border>
       <left/>
       <right/>
@@ -491,6 +537,58 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -499,26 +597,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -535,38 +615,59 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
@@ -574,52 +675,69 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -900,10 +1018,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:K28"/>
+  <dimension ref="B1:P34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,388 +1032,529 @@
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" customWidth="1"/>
     <col min="7" max="7" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" customWidth="1"/>
     <col min="10" max="10" width="10.28515625" customWidth="1"/>
     <col min="11" max="11" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="33"/>
+    </row>
+    <row r="3" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="35"/>
+      <c r="D4" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="18"/>
-      <c r="H4" s="31" t="s">
+      <c r="E4" s="36"/>
+      <c r="F4" s="9"/>
+      <c r="H4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="33" t="s">
+      <c r="J4" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="9">
+    <row r="5" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
         <v>336</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="1">
         <v>225</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="18"/>
-      <c r="H5" s="20" t="s">
+      <c r="F5" s="9"/>
+      <c r="H5" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="16"/>
-      <c r="J5" s="21"/>
-    </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
+      <c r="I5" s="51"/>
+      <c r="J5" s="52"/>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="N5" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="3">
         <v>438</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="1">
         <v>373</v>
       </c>
-      <c r="E6" s="19" t="s">
+      <c r="E6" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="19"/>
-      <c r="G6" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="34" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J6" s="36"/>
-    </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
+      <c r="J6" s="17"/>
+      <c r="L6" s="25"/>
+      <c r="M6" s="26"/>
+      <c r="N6" s="26"/>
+      <c r="O6" s="26"/>
+      <c r="P6" s="26"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="3">
         <v>555</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="1">
         <v>487</v>
       </c>
-      <c r="E7" s="19" t="s">
+      <c r="E7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="19"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="37" t="s">
+      <c r="F7" s="10"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J7" s="38"/>
-    </row>
-    <row r="8" spans="2:11" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="9">
+      <c r="J7" s="19"/>
+      <c r="L7" s="25"/>
+      <c r="M7" s="26"/>
+      <c r="N7" s="26"/>
+      <c r="O7" s="26"/>
+      <c r="P7" s="26"/>
+    </row>
+    <row r="8" spans="2:16" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3">
         <v>814</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="1">
         <v>502</v>
       </c>
-      <c r="E8" s="19" t="s">
+      <c r="E8" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="19"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="37" t="s">
+      <c r="F8" s="10"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="38"/>
+      <c r="J8" s="19"/>
       <c r="K8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="45" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="9"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="7">
+      <c r="M8" s="26"/>
+      <c r="N8" s="26"/>
+      <c r="O8" s="26"/>
+      <c r="P8" s="26"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="3"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="1">
         <v>657</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="H9" s="37" t="s">
+      <c r="F9" s="9"/>
+      <c r="G9" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="H9" s="43" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="44" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="38" t="s">
+      <c r="J9" s="46" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="10"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="8">
+      <c r="L9" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="O9" s="26"/>
+      <c r="P9" s="26"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="2">
         <v>673</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="18"/>
-      <c r="G10" s="28"/>
-      <c r="H10" s="37" t="s">
+      <c r="F10" s="9"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="38" t="s">
+      <c r="J10" s="19" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G11" s="28"/>
-      <c r="H11" s="37" t="s">
+      <c r="L10" s="25"/>
+      <c r="M10" s="26"/>
+      <c r="N10" s="26"/>
+      <c r="O10" s="26"/>
+      <c r="P10" s="26"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G11" s="27"/>
+      <c r="H11" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="I11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J11" s="38" t="s">
+      <c r="J11" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G12" s="28"/>
-      <c r="H12" s="37" t="s">
+      <c r="L11" s="25"/>
+      <c r="M11" s="26"/>
+      <c r="N11" s="26"/>
+      <c r="O11" s="26"/>
+      <c r="P11" s="26"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G12" s="27"/>
+      <c r="H12" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I12" s="13" t="s">
+      <c r="I12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J12" s="38" t="s">
+      <c r="J12" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G13" s="28"/>
-      <c r="H13" s="37" t="s">
+      <c r="L12" s="25"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
+      <c r="O12" s="26"/>
+      <c r="P12" s="26"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G13" s="27"/>
+      <c r="H13" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="13" t="s">
+      <c r="I13" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J13" s="38" t="s">
+      <c r="J13" s="19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G14" s="28"/>
-      <c r="H14" s="37" t="s">
+      <c r="L13" s="25"/>
+      <c r="M13" s="26"/>
+      <c r="N13" s="26"/>
+      <c r="O13" s="26"/>
+      <c r="P13" s="26"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G14" s="27"/>
+      <c r="H14" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="13" t="s">
+      <c r="I14" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="38" t="s">
+      <c r="J14" s="19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G15" s="29"/>
-      <c r="H15" s="22" t="s">
+      <c r="L14" s="25"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G15" s="11"/>
+      <c r="H15" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="17"/>
-      <c r="J15" s="23"/>
-    </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="G16" s="29"/>
-      <c r="H16" s="24" t="s">
+      <c r="I15" s="38"/>
+      <c r="J15" s="39"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="G16" s="11"/>
+      <c r="H16" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="I16" s="15"/>
-      <c r="J16" s="25"/>
-    </row>
-    <row r="17" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G17" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="H17" s="39" t="s">
+      <c r="I16" s="41"/>
+      <c r="J16" s="42"/>
+    </row>
+    <row r="17" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G17" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" s="19"/>
+      <c r="L17" s="45"/>
+      <c r="M17" s="26"/>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+    </row>
+    <row r="18" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G18" s="27"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" s="19"/>
+      <c r="L18" s="45"/>
+      <c r="M18" s="26"/>
+      <c r="N18" s="26"/>
+      <c r="O18" s="26"/>
+      <c r="P18" s="26"/>
+    </row>
+    <row r="19" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G19" s="27"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J19" s="19"/>
+      <c r="L19" s="45"/>
+      <c r="M19" s="26"/>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+    </row>
+    <row r="20" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G20" s="27"/>
+      <c r="H20" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="J20" s="19"/>
+      <c r="L20" s="45"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+    </row>
+    <row r="21" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G21" s="27"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" s="19"/>
+      <c r="L21" s="45"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+    </row>
+    <row r="22" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G22" s="27"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J22" s="19"/>
+      <c r="L22" s="45"/>
+      <c r="M22" s="26"/>
+      <c r="N22" s="26"/>
+      <c r="O22" s="26"/>
+      <c r="P22" s="26"/>
+    </row>
+    <row r="23" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G23" s="11"/>
+      <c r="H23" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="I23" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J23" s="53"/>
+      <c r="L23" s="45"/>
+      <c r="M23" s="26"/>
+      <c r="N23" s="26"/>
+      <c r="O23" s="26"/>
+      <c r="P23" s="26"/>
+    </row>
+    <row r="24" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G24" s="11"/>
+      <c r="H24" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="53"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="26"/>
+      <c r="O24" s="26"/>
+      <c r="P24" s="26"/>
+    </row>
+    <row r="25" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G25" s="11"/>
+      <c r="H25" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="I25" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J25" s="53"/>
+      <c r="L25" s="45"/>
+      <c r="M25" s="26"/>
+      <c r="N25" s="26"/>
+      <c r="O25" s="26"/>
+      <c r="P25" s="26"/>
+    </row>
+    <row r="26" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G26" s="11"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="J26" s="53"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="26"/>
+      <c r="N26" s="26"/>
+      <c r="O26" s="26"/>
+      <c r="P26" s="26"/>
+    </row>
+    <row r="27" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G27" s="11"/>
+      <c r="H27" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="I27" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J27" s="53"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="26"/>
+      <c r="O27" s="26"/>
+      <c r="P27" s="26"/>
+    </row>
+    <row r="28" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G28" s="11"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="J28" s="53"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="26"/>
+      <c r="N28" s="26"/>
+      <c r="O28" s="26"/>
+      <c r="P28" s="26"/>
+    </row>
+    <row r="29" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G29" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="38"/>
-    </row>
-    <row r="18" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G18" s="28"/>
-      <c r="H18" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="I18" s="40" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="38"/>
-    </row>
-    <row r="19" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G19" s="28"/>
-      <c r="H19" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="I19" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="J19" s="38"/>
-    </row>
-    <row r="20" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G20" s="28"/>
-      <c r="H20" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="I20" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="J20" s="38"/>
-    </row>
-    <row r="21" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G21" s="28"/>
-      <c r="H21" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="J21" s="38"/>
-    </row>
-    <row r="22" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G22" s="28"/>
-      <c r="H22" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="J22" s="38"/>
-    </row>
-    <row r="23" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G23" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="H23" s="39" t="s">
-        <v>25</v>
-      </c>
-      <c r="I23" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G24" s="28"/>
-      <c r="H24" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="I24" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="25" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G25" s="28"/>
-      <c r="H25" s="39" t="s">
-        <v>27</v>
-      </c>
-      <c r="I25" s="40" t="s">
-        <v>17</v>
-      </c>
-      <c r="J25" s="38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G26" s="28"/>
-      <c r="H26" s="39" t="s">
-        <v>28</v>
-      </c>
-      <c r="I26" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="38" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="7:10" x14ac:dyDescent="0.25">
-      <c r="G27" s="28"/>
-      <c r="H27" s="39" t="s">
-        <v>29</v>
-      </c>
-      <c r="I27" s="40" t="s">
-        <v>19</v>
-      </c>
-      <c r="J27" s="38" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G28" s="30"/>
-      <c r="H28" s="41" t="s">
-        <v>30</v>
-      </c>
-      <c r="I28" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="J28" s="43" t="s">
-        <v>18</v>
-      </c>
+      <c r="H29" s="49"/>
+      <c r="I29" s="48"/>
+      <c r="J29" s="46"/>
+    </row>
+    <row r="30" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G30" s="27"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="48"/>
+      <c r="J30" s="46"/>
+    </row>
+    <row r="31" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G31" s="27"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="19"/>
+    </row>
+    <row r="32" spans="7:16" x14ac:dyDescent="0.25">
+      <c r="G32" s="27"/>
+      <c r="H32" s="20"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="19"/>
+    </row>
+    <row r="33" spans="7:10" x14ac:dyDescent="0.25">
+      <c r="G33" s="27"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="19"/>
+    </row>
+    <row r="34" spans="7:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="28"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="G23:G28"/>
+    <mergeCell ref="G29:G34"/>
     <mergeCell ref="G9:G14"/>
     <mergeCell ref="G17:G22"/>
     <mergeCell ref="G6:G8"/>

</xml_diff>